<commit_message>
Updated Manual, UI Concepts, and Project Timeline
</commit_message>
<xml_diff>
--- a/DOCS/Illuminati_Gantt_Timeline.xlsx
+++ b/DOCS/Illuminati_Gantt_Timeline.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>ACTIVITY</t>
   </si>
@@ -80,9 +80,6 @@
     <t>FlowCharts</t>
   </si>
   <si>
-    <t>Concept Art</t>
-  </si>
-  <si>
     <t>Phase IV: Implementation &amp; Debugging</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>N, M, J</t>
   </si>
   <si>
-    <t>M, J</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -129,6 +123,9 @@
   </si>
   <si>
     <t>Gameplay Rules, Testcases, and Functionality</t>
+  </si>
+  <si>
+    <t>N, J</t>
   </si>
 </sst>
 </file>
@@ -544,7 +541,572 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="59">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1064,10 +1626,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:O26"/>
+  <dimension ref="B1:O25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1095,7 +1657,7 @@
     </row>
     <row r="2" spans="2:15" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="9"/>
       <c r="E2" s="5"/>
@@ -1223,7 +1785,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="12"/>
@@ -1243,7 +1805,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
@@ -1263,7 +1825,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="12"/>
@@ -1283,7 +1845,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="12"/>
@@ -1361,7 +1923,7 @@
       <c r="C13" s="12"/>
       <c r="D13" s="12"/>
       <c r="E13" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -1381,7 +1943,7 @@
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -1402,12 +1964,10 @@
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
@@ -1416,7 +1976,7 @@
     </row>
     <row r="16" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
@@ -1424,17 +1984,19 @@
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
       <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
@@ -1442,13 +2004,13 @@
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="13" t="s">
-        <v>25</v>
-      </c>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+      <c r="M17" s="13" t="s">
+        <v>29</v>
+      </c>
       <c r="N17" s="14"/>
       <c r="O17" s="12"/>
     </row>
@@ -1464,11 +2026,11 @@
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
-      <c r="K18" s="14" t="s">
-        <v>28</v>
-      </c>
+      <c r="K18" s="12"/>
       <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
+      <c r="M18" s="13" t="s">
+        <v>26</v>
+      </c>
       <c r="N18" s="14"/>
       <c r="O18" s="12"/>
     </row>
@@ -1485,10 +2047,8 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
-      <c r="L19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="13"/>
       <c r="N19" s="14"/>
       <c r="O19" s="12"/>
     </row>
@@ -1496,43 +2056,41 @@
       <c r="B20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14" t="s">
-        <v>25</v>
-      </c>
+      <c r="C20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
-      <c r="O20" s="12"/>
+      <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
     </row>
-    <row r="22" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="8" t="s">
         <v>20</v>
       </c>
@@ -1547,10 +2105,12 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
+      <c r="N22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" s="14"/>
     </row>
-    <row r="23" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1565,8 +2125,8 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="N23" s="14" t="s">
-        <v>25</v>
+      <c r="N23" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="O23" s="14"/>
     </row>
@@ -1585,112 +2145,196 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
-      <c r="N24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="O24" s="14"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="13" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="25" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:O10 D15:O16 D13:D14 F13:O14 D12:O12 E11:O11 D18:O25 D17:J17 L17:O17">
-    <cfRule type="expression" dxfId="18" priority="1">
+  <conditionalFormatting sqref="D15:O15 D13:D14 F13:O14 D12:O12 E11:O11 D20:O21 D16:J16 L16:O16 D17:K18 D24:N24 D22:M23 O22:O23 C10:C19 D5:O10 N17:O19 D19:J19">
+    <cfRule type="expression" dxfId="58" priority="41">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="3">
+    <cfRule type="expression" dxfId="57" priority="43">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="56" priority="44">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="55" priority="45">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="54" priority="46">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7">
-      <formula>D$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="53" priority="47">
+      <formula>C$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="52" priority="51">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:D26">
-    <cfRule type="expression" dxfId="10" priority="2">
+  <conditionalFormatting sqref="C25:D25">
+    <cfRule type="expression" dxfId="50" priority="42">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:O4">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="49" priority="48">
       <formula>D$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5 C10:C20 C22:C25">
-    <cfRule type="expression" dxfId="8" priority="21">
+  <conditionalFormatting sqref="C5 C21:C24">
+    <cfRule type="expression" dxfId="48" priority="61">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="22">
+    <cfRule type="expression" dxfId="47" priority="62">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="23">
+    <cfRule type="expression" dxfId="46" priority="63">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="24">
+    <cfRule type="expression" dxfId="45" priority="64">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="25">
+    <cfRule type="expression" dxfId="44" priority="65">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="26">
+    <cfRule type="expression" dxfId="43" priority="66">
       <formula>C$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="27">
+    <cfRule type="expression" dxfId="42" priority="67">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="28">
+    <cfRule type="expression" dxfId="41" priority="68">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="0" priority="32">
+    <cfRule type="expression" dxfId="40" priority="72">
       <formula>C$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="405" yWindow="525" count="7">
+  <conditionalFormatting sqref="L17">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>L$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>L$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>L$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>K$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations xWindow="794" yWindow="665" count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="C2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="E2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="K2 E13:E14 C6:C9 D11 K17 C21"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="K2 E13:E14 C6:C9 D11 K16 C20 M17:M19 N22:N23 O24"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2"/>

</xml_diff>